<commit_message>
Adding Matrix and Arrays Problems
</commit_message>
<xml_diff>
--- a/Arrays/Problems.xlsx
+++ b/Arrays/Problems.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Array Rotations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="325">
   <si>
     <t>1. Program for array rotation</t>
   </si>
@@ -1067,9 +1067,6 @@
     <t>1. Shortest Un-ordered Subarray</t>
   </si>
   <si>
-    <t>2. Shortest Un-ordered Subarray</t>
-  </si>
-  <si>
     <t>You know the method of getting the index of last occurance of an element - index of first occurance of an element in O(logn).</t>
   </si>
   <si>
@@ -1101,6 +1098,141 @@
   </si>
   <si>
     <t>Amazon, Google, Microsoft</t>
+  </si>
+  <si>
+    <t>You know the approach now</t>
+  </si>
+  <si>
+    <t>You have done this using Segmenet Tree</t>
+  </si>
+  <si>
+    <t>using segment tree</t>
+  </si>
+  <si>
+    <t>it has some other solution, you need to review this</t>
+  </si>
+  <si>
+    <t>Review,</t>
+  </si>
+  <si>
+    <t>this is the awesomest approach seen so far</t>
+  </si>
+  <si>
+    <t>find peak element, done on local</t>
+  </si>
+  <si>
+    <t>Easy to implement, no need to do</t>
+  </si>
+  <si>
+    <t>done in range queries folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">done </t>
+  </si>
+  <si>
+    <t>its done on leetcode.</t>
+  </si>
+  <si>
+    <t>another variation of above problem</t>
+  </si>
+  <si>
+    <t>its done in local, with the variation of -ve numbers as well.</t>
+  </si>
+  <si>
+    <t>undone</t>
+  </si>
+  <si>
+    <t>incomplete, there is something missing in solution</t>
+  </si>
+  <si>
+    <t>done in local, it’s a simple approach of Binary Search</t>
+  </si>
+  <si>
+    <t>its done in local, using hashmap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Done </t>
+  </si>
+  <si>
+    <t>using hashing, it has a nice approach</t>
+  </si>
+  <si>
+    <t>don</t>
+  </si>
+  <si>
+    <t>need to review this algorithm. Not clear when implemented</t>
+  </si>
+  <si>
+    <t>Its done, but you need to review this algorithm. It uses some trick of intersection between, 2 arrays.</t>
+  </si>
+  <si>
+    <t>Its done, with the best possible solution given on interview bit.</t>
+  </si>
+  <si>
+    <t>Not clear, need to discuss this algorithm</t>
+  </si>
+  <si>
+    <t>done on interviewbit : https://www.interviewbit.com/problems/remove-element-from-array/</t>
+  </si>
+  <si>
+    <t>Its done in local, nice approach you know it better.</t>
+  </si>
+  <si>
+    <t>Very unique approach, rethink it again. Using Xor</t>
+  </si>
+  <si>
+    <t>Amazon interview question</t>
+  </si>
+  <si>
+    <t>if the array is infinite and sorted, then first you have to find the bounds. Now to find the bounds iterate the loop in power of 2. once you reached to the value greater then the key. Fix the bound over there and then apply the binary search.</t>
+  </si>
+  <si>
+    <t>using hashing, it has a nice approach, key become element and value is the position</t>
+  </si>
+  <si>
+    <t>Solution is easy, but not worth to implement.</t>
+  </si>
+  <si>
+    <t>Done using hashing you know the solution</t>
+  </si>
+  <si>
+    <t>you know the better solution, no need to implement</t>
+  </si>
+  <si>
+    <t>Irrevelant Question, rethink again</t>
+  </si>
+  <si>
+    <t>Simple Transformation question it is</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Microsoft</t>
+  </si>
+  <si>
+    <t>you know the solution,</t>
+  </si>
+  <si>
+    <t>same algorithm</t>
+  </si>
+  <si>
+    <t>It has a proper algorithm, you need to remember it.</t>
+  </si>
+  <si>
+    <t>Its easy to implement you know the solution</t>
+  </si>
+  <si>
+    <t>Amazon, Citrix, DE Shaw, Informatica, Microsoft, Ola, One97, Opera, Paytm, Snapdeal, Streamoid Technologi, Visa</t>
+  </si>
+  <si>
+    <t>It’s a simple logic, you can do it next time</t>
+  </si>
+  <si>
+    <t>The concept is simple, you have to first create the magic square and later on you have to swap the diagonal elements for more clearification go to the link.</t>
+  </si>
+  <si>
+    <t>Its simple no need to implement</t>
+  </si>
+  <si>
+    <t>Its simple think of it doing using HashMap</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -1271,6 +1403,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1958,7 +2093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -2414,12 +2549,13 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="75.140625" customWidth="1"/>
+    <col min="1" max="1" width="97.42578125" customWidth="1"/>
+    <col min="3" max="3" width="68.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2437,46 +2573,94 @@
       <c r="A3" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="B3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="B4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C4" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="B5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="B6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="C7" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="C8" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="B9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="B10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C10" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="B11" t="s">
+        <v>199</v>
+      </c>
+      <c r="C11" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -2492,25 +2676,49 @@
       <c r="A14" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="B14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="B15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C17" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>95</v>
+      </c>
+      <c r="B18" t="s">
+        <v>199</v>
+      </c>
+      <c r="C18" t="s">
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -2541,12 +2749,13 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="97.7109375" customWidth="1"/>
+    <col min="3" max="3" width="56.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2563,6 +2772,12 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>96</v>
+      </c>
+      <c r="B3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2653,10 +2868,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2972,7 +3187,7 @@
         <v>186</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D26" s="10"/>
     </row>
@@ -2992,7 +3207,7 @@
         <v>186</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D28" s="10"/>
     </row>
@@ -3004,7 +3219,7 @@
         <v>186</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D29" s="10"/>
     </row>
@@ -3015,15 +3230,19 @@
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
+      <c r="B31" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3038,8 +3257,12 @@
       <c r="A33" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
+      <c r="B33" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>295</v>
+      </c>
       <c r="D33" s="10"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3054,24 +3277,36 @@
       <c r="A35" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
+      <c r="B35" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>296</v>
+      </c>
       <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
+      <c r="B36" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>298</v>
+      </c>
       <c r="D36" s="10"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
+      <c r="B37" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>300</v>
+      </c>
       <c r="D37" s="10"/>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3082,7 +3317,7 @@
         <v>186</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D38" s="10"/>
     </row>
@@ -3094,7 +3329,7 @@
         <v>186</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D39" s="10"/>
     </row>
@@ -3106,12 +3341,16 @@
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
+      <c r="B41" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>301</v>
+      </c>
       <c r="D41" s="10"/>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3122,26 +3361,36 @@
         <v>186</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
+      <c r="B44" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>309</v>
+      </c>
       <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3152,7 +3401,7 @@
         <v>186</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D45" s="10"/>
     </row>
@@ -3164,34 +3413,46 @@
         <v>186</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
+      <c r="B47" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>304</v>
+      </c>
       <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
+      <c r="B48" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>305</v>
+      </c>
       <c r="D48" s="10"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
+      <c r="B49" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>302</v>
+      </c>
       <c r="D49" s="10"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3202,28 +3463,34 @@
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+    <row r="51" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>160</v>
       </c>
       <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
+      <c r="C52" s="10" t="s">
+        <v>310</v>
+      </c>
       <c r="D52" s="10"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
+      <c r="B53" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>306</v>
+      </c>
       <c r="D53" s="10"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3231,38 +3498,54 @@
         <v>162</v>
       </c>
       <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
+      <c r="C54" s="10" t="s">
+        <v>303</v>
+      </c>
       <c r="D54" s="10"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>265</v>
       </c>
+      <c r="C55" s="10" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>269</v>
-      </c>
+      <c r="A59" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3321,33 +3604,33 @@
     <hyperlink ref="D10" r:id="rId53" display="https://practice.geeksforgeeks.org/company/Payu/"/>
     <hyperlink ref="D22" r:id="rId54" display="https://practice.geeksforgeeks.org/company/MAQ Software/"/>
     <hyperlink ref="A55" r:id="rId55" display="https://www.geeksforgeeks.org/searching-array-adjacent-differ-k/"/>
-    <hyperlink ref="A56" r:id="rId56" display="https://www.geeksforgeeks.org/searching-array-adjacent-differ-k/"/>
-    <hyperlink ref="A57" r:id="rId57" display="https://www.geeksforgeeks.org/maximum-subarray-sum-excluding-certain-elements/"/>
-    <hyperlink ref="A58" r:id="rId58" display="https://www.geeksforgeeks.org/find-repetitive-element-1-n-1/"/>
-    <hyperlink ref="A59" r:id="rId59" display="https://www.geeksforgeeks.org/shortest-un-ordered-subarray/"/>
-    <hyperlink ref="A60" r:id="rId60" display="https://www.geeksforgeeks.org/shortest-un-ordered-subarray/"/>
-    <hyperlink ref="D42" r:id="rId61" display="https://practice.geeksforgeeks.org/company/Oracle/"/>
+    <hyperlink ref="A56" r:id="rId56" display="https://www.geeksforgeeks.org/maximum-subarray-sum-excluding-certain-elements/"/>
+    <hyperlink ref="A57" r:id="rId57" display="https://www.geeksforgeeks.org/find-repetitive-element-1-n-1/"/>
+    <hyperlink ref="A58" r:id="rId58" display="https://www.geeksforgeeks.org/shortest-un-ordered-subarray/"/>
+    <hyperlink ref="D42" r:id="rId59" display="https://practice.geeksforgeeks.org/company/Oracle/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId62"/>
+  <pageSetup orientation="portrait" r:id="rId60"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="86.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="1" max="1" width="70.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="72.140625" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -3358,79 +3641,139 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" t="s">
+        <v>321</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C16" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>177</v>
+      </c>
+      <c r="B17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>